<commit_message>
fixed effects, lag/lead, FWL
</commit_message>
<xml_diff>
--- a/Data/elasticnetBetas.xlsx
+++ b/Data/elasticnetBetas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrymanley/Desktop/Research/googletrends/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D631A8B-E9A8-CF48-B2E0-7CFE41DA04BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36A688C-637A-8D47-B155-C3F60F7C3752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="460" windowWidth="19960" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3020" yWindow="460" windowWidth="25780" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,25 +515,25 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.2674361179521844E-2</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-7.9631167749406059E-4</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-5.1132014932122084E-3</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -548,63 +548,63 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>-3.1575289047638452E-3</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>-5.3933750179314703E-3</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>-1.3674654575419123E-2</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>-2.6648057095999184E-2</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-1.0740643434496216E-2</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1.9344978586113499E-3</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>9.0783844370830435E-3</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>9.8194726894650797E-3</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>2.3994456005854568E-2</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>6.9188130498206437</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>0.96653764279594856</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1.2674361179521844E-2</v>
+        <v>9.5398951109139929E-3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-7.9631167749406059E-4</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>-5.1132014932122084E-3</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -613,63 +613,63 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>-3.5326466365490825E-3</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>-3.1575289047638452E-3</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>-5.3933750179314703E-3</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>-1.3674654575419123E-2</v>
+        <v>-4.4760922426999488E-3</v>
       </c>
       <c r="O3">
-        <v>-2.6648057095999184E-2</v>
+        <v>-2.3237540705029749E-3</v>
       </c>
       <c r="P3">
-        <v>-1.0740643434496216E-2</v>
+        <v>-1.7337832876794951E-3</v>
       </c>
       <c r="Q3">
-        <v>1.9344978586113499E-3</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>9.0783844370830435E-3</v>
+        <v>-1.0860523002064967E-3</v>
       </c>
       <c r="S3">
-        <v>9.8194726894650797E-3</v>
+        <v>3.8803406329340558E-3</v>
       </c>
       <c r="T3">
-        <v>2.3994456005854568E-2</v>
+        <v>3.854300544224806E-3</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>6.9188130498206437</v>
+        <v>6.4014515297961081</v>
       </c>
       <c r="W3">
-        <v>0.96653764279594856</v>
+        <v>0.7479935036399401</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>9.5398951109139929E-3</v>
+        <v>1.8154945468296144E-2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2.3423732543468956E-3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-7.4779651364991137E-3</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -678,13 +678,13 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>5.6798764609264328E-3</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>-3.5326466365490825E-3</v>
+        <v>-1.5121040312440468E-2</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -693,54 +693,54 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>7.1837835405612876E-3</v>
       </c>
       <c r="N4">
-        <v>-4.4760922426999488E-3</v>
+        <v>-2.0972173243984722E-3</v>
       </c>
       <c r="O4">
-        <v>-2.3237540705029749E-3</v>
+        <v>-4.1682844166016945E-3</v>
       </c>
       <c r="P4">
-        <v>-1.7337832876794951E-3</v>
+        <v>-1.6404703903172311E-2</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>7.1994697958083845E-3</v>
       </c>
       <c r="R4">
-        <v>-1.0860523002064967E-3</v>
+        <v>1.4153223436466017E-2</v>
       </c>
       <c r="S4">
-        <v>3.8803406329340558E-3</v>
+        <v>1.5309514391809805E-2</v>
       </c>
       <c r="T4">
-        <v>3.854300544224806E-3</v>
+        <v>1.9130653699567488E-2</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>-3.3528720613227887E-3</v>
       </c>
       <c r="V4">
-        <v>6.4014515297961081</v>
+        <v>4.659744305859908</v>
       </c>
       <c r="W4">
-        <v>0.7479935036399401</v>
+        <v>0.97167939948284732</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1.8154945468296144E-2</v>
+        <v>1.398751511444095E-2</v>
       </c>
       <c r="D5">
-        <v>2.3423732543468956E-3</v>
+        <v>1.5930378183967153E-3</v>
       </c>
       <c r="E5">
-        <v>-7.4779651364991137E-3</v>
+        <v>-1.4027146487879765E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -749,69 +749,69 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>5.6798764609264328E-3</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>-1.5121040312440468E-2</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3.7260829299627083E-3</v>
       </c>
       <c r="M5">
-        <v>7.1837835405612876E-3</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>-2.0972173243984722E-3</v>
+        <v>1.2899601257757602E-2</v>
       </c>
       <c r="O5">
-        <v>-4.1682844166016945E-3</v>
+        <v>-2.2973723810181448E-2</v>
       </c>
       <c r="P5">
-        <v>-1.6404703903172311E-2</v>
+        <v>-9.7484445714981563E-3</v>
       </c>
       <c r="Q5">
-        <v>7.1994697958083845E-3</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1.4153223436466017E-2</v>
+        <v>5.0513806099026982E-2</v>
       </c>
       <c r="S5">
-        <v>1.5309514391809805E-2</v>
+        <v>7.4204523739220081E-3</v>
       </c>
       <c r="T5">
-        <v>1.9130653699567488E-2</v>
+        <v>1.3527074359121847E-2</v>
       </c>
       <c r="U5">
-        <v>-3.3528720613227887E-3</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>4.659744305859908</v>
+        <v>2.8082103999843619</v>
       </c>
       <c r="W5">
-        <v>0.97167939948284732</v>
+        <v>0.95222101094632727</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1.2358764246219721E-2</v>
       </c>
       <c r="C6">
-        <v>1.398751511444095E-2</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1.5930378183967153E-3</v>
+        <v>1.5914420504785118E-3</v>
       </c>
       <c r="E6">
-        <v>-1.4027146487879765E-2</v>
+        <v>-6.5416788760971371E-3</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -820,146 +820,146 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>3.9721777602490021E-3</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>-8.0244370980156292E-3</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>3.7260829299627083E-3</v>
+        <v>-2.9642865908144231E-2</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>-2.022817996636176E-3</v>
       </c>
       <c r="N6">
-        <v>1.2899601257757602E-2</v>
+        <v>-1.4357994865540348E-2</v>
       </c>
       <c r="O6">
-        <v>-2.2973723810181448E-2</v>
+        <v>3.1582929938141449E-2</v>
       </c>
       <c r="P6">
-        <v>-9.7484445714981563E-3</v>
+        <v>-2.7675276566863659E-2</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1.3025141372366959E-2</v>
       </c>
       <c r="R6">
-        <v>5.0513806099026982E-2</v>
+        <v>3.5317540757024084E-2</v>
       </c>
       <c r="S6">
-        <v>7.4204523739220081E-3</v>
+        <v>1.0493696742628168E-2</v>
       </c>
       <c r="T6">
-        <v>1.3527074359121847E-2</v>
+        <v>3.6248465127139723E-2</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>-1.1820708974485554E-2</v>
       </c>
       <c r="V6">
-        <v>2.8082103999843619</v>
+        <v>3.4427767820375603</v>
       </c>
       <c r="W6">
-        <v>0.95222101094632727</v>
+        <v>0.9860101105491248</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>1.2358764246219721E-2</v>
+        <v>4.2642409537672326E-3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2.9979670877879096E-2</v>
       </c>
       <c r="D7">
-        <v>1.5914420504785118E-3</v>
+        <v>5.7974095450683922E-3</v>
       </c>
       <c r="E7">
-        <v>-6.5416788760971371E-3</v>
+        <v>-1.0378348920734753E-2</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-3.8328251325559699E-3</v>
       </c>
       <c r="H7">
-        <v>3.9721777602490021E-3</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>-8.0244370980156292E-3</v>
+        <v>-1.3183240614562606E-2</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>-2.9642865908144231E-2</v>
+        <v>-1.7401687580101733E-2</v>
       </c>
       <c r="M7">
-        <v>-2.022817996636176E-3</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>-1.4357994865540348E-2</v>
+        <v>1.3027532733492758E-2</v>
       </c>
       <c r="O7">
-        <v>3.1582929938141449E-2</v>
+        <v>2.246386898946354E-2</v>
       </c>
       <c r="P7">
-        <v>-2.7675276566863659E-2</v>
+        <v>-3.6856828529776009E-2</v>
       </c>
       <c r="Q7">
-        <v>1.3025141372366959E-2</v>
+        <v>3.0761685904394228E-3</v>
       </c>
       <c r="R7">
-        <v>3.5317540757024084E-2</v>
+        <v>4.9548735399423276E-2</v>
       </c>
       <c r="S7">
-        <v>1.0493696742628168E-2</v>
+        <v>2.5371204110746448E-2</v>
       </c>
       <c r="T7">
-        <v>3.6248465127139723E-2</v>
+        <v>8.2742956474633547E-3</v>
       </c>
       <c r="U7">
-        <v>-1.1820708974485554E-2</v>
+        <v>-8.898674833939791E-3</v>
       </c>
       <c r="V7">
-        <v>3.4427767820375603</v>
+        <v>-0.19878715025018856</v>
       </c>
       <c r="W7">
-        <v>0.9860101105491248</v>
+        <v>0.956876244858757</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>4.2642409537672326E-3</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>2.9979670877879096E-2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>5.7974095450683922E-3</v>
+        <v>-5.9125373621809222E-3</v>
       </c>
       <c r="E8">
-        <v>-1.0378348920734753E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>-3.8328251325559699E-3</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -968,51 +968,51 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>-1.3183240614562606E-2</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>-1.7401687580101733E-2</v>
+        <v>-6.6525582936491278E-3</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1.3027532733492758E-2</v>
+        <v>-5.7939022823001044E-3</v>
       </c>
       <c r="O8">
-        <v>2.246386898946354E-2</v>
+        <v>1.0297034207577091E-2</v>
       </c>
       <c r="P8">
-        <v>-3.6856828529776009E-2</v>
+        <v>-1.6865427276479331E-2</v>
       </c>
       <c r="Q8">
-        <v>3.0761685904394228E-3</v>
+        <v>4.5364928746598077E-3</v>
       </c>
       <c r="R8">
-        <v>4.9548735399423276E-2</v>
+        <v>4.0126703867025701E-2</v>
       </c>
       <c r="S8">
-        <v>2.5371204110746448E-2</v>
+        <v>1.0823258779791173E-2</v>
       </c>
       <c r="T8">
-        <v>8.2742956474633547E-3</v>
+        <v>2.014520973058808E-2</v>
       </c>
       <c r="U8">
-        <v>-8.898674833939791E-3</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>-0.19878715025018856</v>
+        <v>3.0771060441112472</v>
       </c>
       <c r="W8">
-        <v>0.956876244858757</v>
+        <v>0.97449215979625414</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-5.9125373621809222E-3</v>
+        <v>1.3207596885524927E-3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1045,57 +1045,57 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>-6.6525582936491278E-3</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>-5.7939022823001044E-3</v>
+        <v>-4.7770374098815979E-3</v>
       </c>
       <c r="O9">
-        <v>1.0297034207577091E-2</v>
+        <v>-8.9563777232429635E-3</v>
       </c>
       <c r="P9">
-        <v>-1.6865427276479331E-2</v>
+        <v>-1.1495935640639309E-2</v>
       </c>
       <c r="Q9">
-        <v>4.5364928746598077E-3</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>4.0126703867025701E-2</v>
+        <v>2.6479665865514711E-2</v>
       </c>
       <c r="S9">
-        <v>1.0823258779791173E-2</v>
+        <v>1.4121423591008098E-2</v>
       </c>
       <c r="T9">
-        <v>2.014520973058808E-2</v>
+        <v>1.8269005129674235E-2</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9">
-        <v>3.0771060441112472</v>
+        <v>3.9749852903735734</v>
       </c>
       <c r="W9">
-        <v>0.97449215979625414</v>
+        <v>0.90812168637991841</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1.3300326696864295E-2</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1.3207596885524927E-3</v>
+        <v>-1.6115193810324762E-2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-1.66851855125696E-2</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1107,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>-1.3017527656082486E-2</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>-1.9011192418630016E-2</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1119,54 +1119,54 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>2.1906996266042526E-2</v>
       </c>
       <c r="N10">
-        <v>-4.7770374098815979E-3</v>
+        <v>-4.061616670282109E-3</v>
       </c>
       <c r="O10">
-        <v>-8.9563777232429635E-3</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>-1.1495935640639309E-2</v>
+        <v>-8.6607317062440334E-3</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>2.6479665865514711E-2</v>
+        <v>1.4897148407328552E-2</v>
       </c>
       <c r="S10">
-        <v>1.4121423591008098E-2</v>
+        <v>2.173724970744928E-2</v>
       </c>
       <c r="T10">
-        <v>1.8269005129674235E-2</v>
+        <v>6.9692337358327385E-3</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>-1.7030747934867864E-3</v>
       </c>
       <c r="V10">
-        <v>3.9749852903735734</v>
+        <v>7.0440962415661916</v>
       </c>
       <c r="W10">
-        <v>0.90812168637991841</v>
+        <v>0.91840220912057846</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1.3300326696864295E-2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.0219757907397174E-2</v>
       </c>
       <c r="D11">
-        <v>-1.6115193810324762E-2</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>-1.66851855125696E-2</v>
+        <v>-2.7910495842208938E-3</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1175,69 +1175,69 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>3.2740928728680731E-3</v>
       </c>
       <c r="I11">
-        <v>-1.3017527656082486E-2</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>-1.9011192418630016E-2</v>
+        <v>-1.5254978193850499E-2</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>-8.6119187904486975E-3</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>3.5581757091157286E-3</v>
       </c>
       <c r="M11">
-        <v>2.1906996266042526E-2</v>
+        <v>6.3532178876726892E-3</v>
       </c>
       <c r="N11">
-        <v>-4.061616670282109E-3</v>
+        <v>-1.544814849595751E-2</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1.532344682919711E-2</v>
       </c>
       <c r="P11">
-        <v>-8.6607317062440334E-3</v>
+        <v>-1.5579634470170434E-2</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>-1.6501842718186476E-4</v>
       </c>
       <c r="R11">
-        <v>1.4897148407328552E-2</v>
+        <v>8.2544660488190653E-3</v>
       </c>
       <c r="S11">
-        <v>2.173724970744928E-2</v>
+        <v>1.1982195070413794E-2</v>
       </c>
       <c r="T11">
-        <v>6.9692337358327385E-3</v>
+        <v>3.7942654214130261E-2</v>
       </c>
       <c r="U11">
-        <v>-1.7030747934867864E-3</v>
+        <v>-8.6390569615799606E-3</v>
       </c>
       <c r="V11">
-        <v>7.0440962415661916</v>
+        <v>4.199775593650557</v>
       </c>
       <c r="W11">
-        <v>0.91840220912057846</v>
+        <v>0.9879220380328444</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>3.9913217283317412E-3</v>
       </c>
       <c r="C12">
-        <v>1.0219757907397174E-2</v>
+        <v>2.3664944769334614E-2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-4.9601649212486264E-3</v>
       </c>
       <c r="E12">
-        <v>-2.7910495842208938E-3</v>
+        <v>-5.940063366717172E-3</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1246,69 +1246,69 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>3.2740928728680731E-3</v>
+        <v>5.0418735710037188E-3</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>-1.5254978193850499E-2</v>
+        <v>-1.252255270587971E-2</v>
       </c>
       <c r="K12">
-        <v>-8.6119187904486975E-3</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>3.5581757091157286E-3</v>
+        <v>-1.048589370212551E-2</v>
       </c>
       <c r="M12">
-        <v>6.3532178876726892E-3</v>
+        <v>2.5395524952437835E-3</v>
       </c>
       <c r="N12">
-        <v>-1.544814849595751E-2</v>
+        <v>-2.5924706728117971E-2</v>
       </c>
       <c r="O12">
-        <v>1.532344682919711E-2</v>
+        <v>3.103759217163421E-2</v>
       </c>
       <c r="P12">
-        <v>-1.5579634470170434E-2</v>
+        <v>-2.4813500968888746E-2</v>
       </c>
       <c r="Q12">
-        <v>-1.6501842718186476E-4</v>
+        <v>-6.9184959258621406E-4</v>
       </c>
       <c r="R12">
-        <v>8.2544660488190653E-3</v>
+        <v>-7.0774181038238465E-3</v>
       </c>
       <c r="S12">
-        <v>1.1982195070413794E-2</v>
+        <v>8.7067623371434762E-3</v>
       </c>
       <c r="T12">
-        <v>3.7942654214130261E-2</v>
+        <v>3.1681721428417846E-2</v>
       </c>
       <c r="U12">
-        <v>-8.6390569615799606E-3</v>
+        <v>-1.3860107037950126E-2</v>
       </c>
       <c r="V12">
-        <v>4.199775593650557</v>
+        <v>5.3804332860435036</v>
       </c>
       <c r="W12">
-        <v>0.9879220380328444</v>
+        <v>0.97304950437174997</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>3.9913217283317412E-3</v>
+        <v>-4.3030233721322621E-3</v>
       </c>
       <c r="C13">
-        <v>2.3664944769334614E-2</v>
+        <v>1.7255971837150282E-2</v>
       </c>
       <c r="D13">
-        <v>-4.9601649212486264E-3</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>-5.940063366717172E-3</v>
+        <v>-1.8401480657446951E-3</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1317,69 +1317,69 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>5.0418735710037188E-3</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>-1.252255270587971E-2</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>-1.048589370212551E-2</v>
+        <v>-6.8639677506119349E-3</v>
       </c>
       <c r="M13">
-        <v>2.5395524952437835E-3</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>-2.5924706728117971E-2</v>
+        <v>8.7520955671409155E-3</v>
       </c>
       <c r="O13">
-        <v>3.103759217163421E-2</v>
+        <v>-7.8287234430313105E-3</v>
       </c>
       <c r="P13">
-        <v>-2.4813500968888746E-2</v>
+        <v>-2.779959683743892E-2</v>
       </c>
       <c r="Q13">
-        <v>-6.9184959258621406E-4</v>
+        <v>1.7601912859474657E-3</v>
       </c>
       <c r="R13">
-        <v>-7.0774181038238465E-3</v>
+        <v>1.7982312579739004E-2</v>
       </c>
       <c r="S13">
-        <v>8.7067623371434762E-3</v>
+        <v>1.1287620515641725E-2</v>
       </c>
       <c r="T13">
-        <v>3.1681721428417846E-2</v>
+        <v>1.9685595408207399E-2</v>
       </c>
       <c r="U13">
-        <v>-1.3860107037950126E-2</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>5.3804332860435036</v>
+        <v>3.1259770203955544</v>
       </c>
       <c r="W13">
-        <v>0.97304950437174997</v>
+        <v>0.92763842169559896</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>-4.3030233721322621E-3</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1.7255971837150282E-2</v>
+        <v>2.7568135662336138E-2</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>-1.8401480657446951E-3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1400,199 +1400,199 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>-6.8639677506119349E-3</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>8.7520955671409155E-3</v>
+        <v>9.1781913945049587E-3</v>
       </c>
       <c r="O14">
-        <v>-7.8287234430313105E-3</v>
+        <v>-3.2013822141480297E-2</v>
       </c>
       <c r="P14">
-        <v>-2.779959683743892E-2</v>
+        <v>-1.6181805160617853E-2</v>
       </c>
       <c r="Q14">
-        <v>1.7601912859474657E-3</v>
+        <v>2.5096872888584814E-3</v>
       </c>
       <c r="R14">
-        <v>1.7982312579739004E-2</v>
+        <v>2.1545533096719111E-2</v>
       </c>
       <c r="S14">
-        <v>1.1287620515641725E-2</v>
+        <v>2.1401126260313333E-2</v>
       </c>
       <c r="T14">
-        <v>1.9685595408207399E-2</v>
+        <v>2.6196898540611548E-2</v>
       </c>
       <c r="U14">
         <v>0</v>
       </c>
       <c r="V14">
-        <v>3.1259770203955544</v>
+        <v>2.8188471552006402</v>
       </c>
       <c r="W14">
-        <v>0.92763842169559896</v>
+        <v>0.91964119920013654</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1.7588902979207928E-3</v>
       </c>
       <c r="C15">
-        <v>2.7568135662336138E-2</v>
+        <v>2.4008139607371547E-2</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>-9.5832056577207989E-3</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1.0019198279625008E-3</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1.0204878841052508E-2</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>-1.6113224055512413E-2</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>9.1129277205296861E-3</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>9.1781913945049587E-3</v>
+        <v>-3.2164743689345021E-2</v>
       </c>
       <c r="O15">
-        <v>-3.2013822141480297E-2</v>
+        <v>3.8237050921295312E-2</v>
       </c>
       <c r="P15">
-        <v>-1.6181805160617853E-2</v>
+        <v>-2.0615101226549463E-2</v>
       </c>
       <c r="Q15">
-        <v>2.5096872888584814E-3</v>
+        <v>1.7250426387590847E-3</v>
       </c>
       <c r="R15">
-        <v>2.1545533096719111E-2</v>
+        <v>-1.0565263610727666E-2</v>
       </c>
       <c r="S15">
-        <v>2.1401126260313333E-2</v>
+        <v>1.4371677992432719E-3</v>
       </c>
       <c r="T15">
-        <v>2.6196898540611548E-2</v>
+        <v>2.5335200153642524E-2</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>-6.232428781878495E-3</v>
       </c>
       <c r="V15">
-        <v>2.8188471552006402</v>
+        <v>4.7575089208070267</v>
       </c>
       <c r="W15">
-        <v>0.91964119920013654</v>
+        <v>0.96381705022167496</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>1.7588902979207928E-3</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>2.4008139607371547E-2</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>-9.5832056577207989E-3</v>
+        <v>-1.0546232761433199E-2</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1.0019198279625008E-3</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1.0204878841052508E-2</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>-1.6113224055512413E-2</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>9.1129277205296861E-3</v>
+        <v>-5.6595590300981234E-3</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>-1.4796185084709587E-3</v>
       </c>
       <c r="N16">
-        <v>-3.2164743689345021E-2</v>
+        <v>6.0265633966364515E-3</v>
       </c>
       <c r="O16">
-        <v>3.8237050921295312E-2</v>
+        <v>3.5976357897432015E-3</v>
       </c>
       <c r="P16">
-        <v>-2.0615101226549463E-2</v>
+        <v>-2.6948415480837914E-2</v>
       </c>
       <c r="Q16">
-        <v>1.7250426387590847E-3</v>
+        <v>7.9302075194426502E-3</v>
       </c>
       <c r="R16">
-        <v>-1.0565263610727666E-2</v>
+        <v>4.3883915540414133E-2</v>
       </c>
       <c r="S16">
-        <v>1.4371677992432719E-3</v>
+        <v>1.7190090724375471E-2</v>
       </c>
       <c r="T16">
-        <v>2.5335200153642524E-2</v>
+        <v>2.1890131185986351E-2</v>
       </c>
       <c r="U16">
-        <v>-6.232428781878495E-3</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>4.7575089208070267</v>
+        <v>3.1070878121171894</v>
       </c>
       <c r="W16">
-        <v>0.96381705022167496</v>
+        <v>0.96455110682223832</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1.4922414232543165E-2</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>-1.0546232761433199E-2</v>
+        <v>-1.4112199956782126E-3</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1607,63 +1607,63 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>-8.8109837748248758E-3</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>-5.6595590300981234E-3</v>
+        <v>2.8156222119279841E-3</v>
       </c>
       <c r="M17">
-        <v>-1.4796185084709587E-3</v>
+        <v>4.4179583407058368E-4</v>
       </c>
       <c r="N17">
-        <v>6.0265633966364515E-3</v>
+        <v>-7.6612997441378285E-3</v>
       </c>
       <c r="O17">
-        <v>3.5976357897432015E-3</v>
+        <v>-1.4549302066571424E-2</v>
       </c>
       <c r="P17">
-        <v>-2.6948415480837914E-2</v>
+        <v>-5.8175741127543552E-3</v>
       </c>
       <c r="Q17">
-        <v>7.9302075194426502E-3</v>
+        <v>1.0996307208793396E-3</v>
       </c>
       <c r="R17">
-        <v>4.3883915540414133E-2</v>
+        <v>1.4045875089670104E-2</v>
       </c>
       <c r="S17">
-        <v>1.7190090724375471E-2</v>
+        <v>-3.8609959606937305E-4</v>
       </c>
       <c r="T17">
-        <v>2.1890131185986351E-2</v>
+        <v>3.6143409072984336E-3</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17">
-        <v>3.1070878121171894</v>
+        <v>3.7820955668919476</v>
       </c>
       <c r="W17">
-        <v>0.96455110682223832</v>
+        <v>0.96645392939193153</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1.4922414232543165E-2</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>-1.4112199956782126E-3</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1678,63 +1678,63 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>-8.8109837748248758E-3</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>2.8156222119279841E-3</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>4.4179583407058368E-4</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>-7.6612997441378285E-3</v>
+        <v>1.6187236555708683E-3</v>
       </c>
       <c r="O18">
-        <v>-1.4549302066571424E-2</v>
+        <v>-1.8903420399204472E-2</v>
       </c>
       <c r="P18">
-        <v>-5.8175741127543552E-3</v>
+        <v>-3.7192876901572403E-3</v>
       </c>
       <c r="Q18">
-        <v>1.0996307208793396E-3</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>1.4045875089670104E-2</v>
+        <v>2.312361978008258E-2</v>
       </c>
       <c r="S18">
-        <v>-3.8609959606937305E-4</v>
+        <v>1.0460433439147633E-2</v>
       </c>
       <c r="T18">
-        <v>3.6143409072984336E-3</v>
+        <v>1.0016101511581641E-2</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18">
-        <v>3.7820955668919476</v>
+        <v>3.831420285466332</v>
       </c>
       <c r="W18">
-        <v>0.96645392939193153</v>
+        <v>0.94832142471057834</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>5.2830362774492802E-3</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1.2456628424249596E-2</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>-6.0672906163033048E-3</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1743,69 +1743,69 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1.6973585294992729E-3</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>-1.6765895203016506E-2</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1.3545577879130841E-2</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>-2.3246925447438882E-3</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>9.6144725125415359E-3</v>
       </c>
       <c r="N19">
-        <v>1.6187236555708683E-3</v>
+        <v>2.6545828821298665E-3</v>
       </c>
       <c r="O19">
-        <v>-1.8903420399204472E-2</v>
+        <v>-2.1436103299535041E-2</v>
       </c>
       <c r="P19">
-        <v>-3.7192876901572403E-3</v>
+        <v>-1.0205266388798491E-2</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>-7.1766345266030432E-4</v>
       </c>
       <c r="R19">
-        <v>2.312361978008258E-2</v>
+        <v>3.0348238821868136E-2</v>
       </c>
       <c r="S19">
-        <v>1.0460433439147633E-2</v>
+        <v>2.3076601464905561E-2</v>
       </c>
       <c r="T19">
-        <v>1.0016101511581641E-2</v>
+        <v>1.8380543093029455E-2</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>-8.0804187048421853E-3</v>
       </c>
       <c r="V19">
-        <v>3.831420285466332</v>
+        <v>4.7609907511303309</v>
       </c>
       <c r="W19">
-        <v>0.94832142471057834</v>
+        <v>0.95263785124788181</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>5.2830362774492802E-3</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>1.2456628424249596E-2</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>-6.0672906163033048E-3</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1814,63 +1814,63 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>1.6973585294992729E-3</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>-1.6765895203016506E-2</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>1.3545577879130841E-2</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>-2.3246925447438882E-3</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>9.6144725125415359E-3</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>2.6545828821298665E-3</v>
+        <v>-8.3799108580610918E-3</v>
       </c>
       <c r="O20">
-        <v>-2.1436103299535041E-2</v>
+        <v>-1.5628111517905382E-2</v>
       </c>
       <c r="P20">
-        <v>-1.0205266388798491E-2</v>
+        <v>-9.0710099644874045E-3</v>
       </c>
       <c r="Q20">
-        <v>-7.1766345266030432E-4</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>3.0348238821868136E-2</v>
+        <v>7.9291114387850872E-3</v>
       </c>
       <c r="S20">
-        <v>2.3076601464905561E-2</v>
+        <v>-8.1919487526793504E-3</v>
       </c>
       <c r="T20">
-        <v>1.8380543093029455E-2</v>
+        <v>1.4929010934439988E-2</v>
       </c>
       <c r="U20">
-        <v>-8.0804187048421853E-3</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>4.7609907511303309</v>
+        <v>7.4352297215157002</v>
       </c>
       <c r="W20">
-        <v>0.95263785124788181</v>
+        <v>0.86138902202208945</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>3.0470505754362678E-2</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1891,63 +1891,63 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>-1.5622561127339649E-2</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>8.0306427886580808E-4</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>-8.3799108580610918E-3</v>
+        <v>3.8286733847799977E-3</v>
       </c>
       <c r="O21">
-        <v>-1.5628111517905382E-2</v>
+        <v>-4.4516393136195083E-3</v>
       </c>
       <c r="P21">
-        <v>-9.0710099644874045E-3</v>
+        <v>-1.7054671564276459E-2</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1.8111954424760138E-3</v>
       </c>
       <c r="R21">
-        <v>7.9291114387850872E-3</v>
+        <v>5.5956358060510372E-2</v>
       </c>
       <c r="S21">
-        <v>-8.1919487526793504E-3</v>
+        <v>1.3726376388901902E-2</v>
       </c>
       <c r="T21">
-        <v>1.4929010934439988E-2</v>
+        <v>8.365972533835522E-3</v>
       </c>
       <c r="U21">
         <v>0</v>
       </c>
       <c r="V21">
-        <v>7.4352297215157002</v>
+        <v>0.55447211278716235</v>
       </c>
       <c r="W21">
-        <v>0.86138902202208945</v>
+        <v>0.94240572513871801</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>-2.8656834399190308E-3</v>
       </c>
       <c r="C22">
-        <v>3.0470505754362678E-2</v>
+        <v>1.2314903907265555E-2</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1.2840512351023309E-3</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-2.9161579568988748E-3</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1956,69 +1956,69 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>4.4625884060369696E-3</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>-1.5622561127339649E-2</v>
+        <v>-1.3986880117915653E-2</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>8.0306427886580808E-4</v>
+        <v>1.9906134797087654E-3</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>8.4553934344107351E-3</v>
       </c>
       <c r="N22">
-        <v>3.8286733847799977E-3</v>
+        <v>-6.9111630270190351E-3</v>
       </c>
       <c r="O22">
-        <v>-4.4516393136195083E-3</v>
+        <v>9.331492604734334E-3</v>
       </c>
       <c r="P22">
-        <v>-1.7054671564276459E-2</v>
+        <v>-5.3142813224920996E-3</v>
       </c>
       <c r="Q22">
-        <v>1.8111954424760138E-3</v>
+        <v>3.5438783703979968E-4</v>
       </c>
       <c r="R22">
-        <v>5.5956358060510372E-2</v>
+        <v>3.0875113659974321E-2</v>
       </c>
       <c r="S22">
-        <v>1.3726376388901902E-2</v>
+        <v>4.458673232332842E-3</v>
       </c>
       <c r="T22">
-        <v>8.365972533835522E-3</v>
+        <v>9.7230420205423797E-3</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>-4.4286993736499924E-3</v>
       </c>
       <c r="V22">
-        <v>0.55447211278716235</v>
+        <v>2.1494136602347855</v>
       </c>
       <c r="W22">
-        <v>0.94240572513871801</v>
+        <v>0.97987389327988106</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23">
-        <v>-2.8656834399190308E-3</v>
+        <v>2.0911183860806855E-3</v>
       </c>
       <c r="C23">
-        <v>1.2314903907265555E-2</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1.2840512351023309E-3</v>
+        <v>2.1443353603603819E-4</v>
       </c>
       <c r="E23">
-        <v>-2.9161579568988748E-3</v>
+        <v>-4.0251525954424772E-3</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2027,72 +2027,72 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>4.4625884060369696E-3</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>-1.3986880117915653E-2</v>
+        <v>-1.403737898729198E-2</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>1.9906134797087654E-3</v>
+        <v>6.3754392885030714E-3</v>
       </c>
       <c r="M23">
-        <v>8.4553934344107351E-3</v>
+        <v>1.1568094662981674E-2</v>
       </c>
       <c r="N23">
-        <v>-6.9111630270190351E-3</v>
+        <v>-5.8354141540474629E-3</v>
       </c>
       <c r="O23">
-        <v>9.331492604734334E-3</v>
+        <v>1.8734684585748899E-2</v>
       </c>
       <c r="P23">
-        <v>-5.3142813224920996E-3</v>
+        <v>-1.2867466220295217E-2</v>
       </c>
       <c r="Q23">
-        <v>3.5438783703979968E-4</v>
+        <v>4.719174345276583E-3</v>
       </c>
       <c r="R23">
-        <v>3.0875113659974321E-2</v>
+        <v>2.4183057192931422E-2</v>
       </c>
       <c r="S23">
-        <v>4.458673232332842E-3</v>
+        <v>2.3987899378312629E-3</v>
       </c>
       <c r="T23">
-        <v>9.7230420205423797E-3</v>
+        <v>1.9275459507501813E-2</v>
       </c>
       <c r="U23">
-        <v>-4.4286993736499924E-3</v>
+        <v>-8.288037763701522E-3</v>
       </c>
       <c r="V23">
-        <v>2.1494136602347855</v>
+        <v>2.3512797903924265</v>
       </c>
       <c r="W23">
-        <v>0.97987389327988106</v>
+        <v>0.9740611796137848</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24">
-        <v>2.0911183860806855E-3</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2.2420285469738347E-2</v>
       </c>
       <c r="D24">
-        <v>2.1443353603603819E-4</v>
+        <v>-1.4443540003761909E-2</v>
       </c>
       <c r="E24">
-        <v>-4.0251525954424772E-3</v>
+        <v>-2.0265201880372693E-3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>8.2535637039212687E-3</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2104,66 +2104,66 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>-1.403737898729198E-2</v>
+        <v>-3.5315671822918442E-2</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>6.3754392885030714E-3</v>
+        <v>7.3502445551724051E-3</v>
       </c>
       <c r="M24">
-        <v>1.1568094662981674E-2</v>
+        <v>1.4243855789215306E-2</v>
       </c>
       <c r="N24">
-        <v>-5.8354141540474629E-3</v>
+        <v>-1.9416698245420239E-2</v>
       </c>
       <c r="O24">
-        <v>1.8734684585748899E-2</v>
+        <v>3.8931888805674206E-2</v>
       </c>
       <c r="P24">
-        <v>-1.2867466220295217E-2</v>
+        <v>-1.4371143568043776E-2</v>
       </c>
       <c r="Q24">
-        <v>4.719174345276583E-3</v>
+        <v>4.611693670466795E-3</v>
       </c>
       <c r="R24">
-        <v>2.4183057192931422E-2</v>
+        <v>3.8105392349912698E-2</v>
       </c>
       <c r="S24">
-        <v>2.3987899378312629E-3</v>
+        <v>1.0261456712862861E-2</v>
       </c>
       <c r="T24">
-        <v>1.9275459507501813E-2</v>
+        <v>2.1803034924040246E-2</v>
       </c>
       <c r="U24">
-        <v>-8.288037763701522E-3</v>
+        <v>-1.5146954018336814E-2</v>
       </c>
       <c r="V24">
-        <v>2.3512797903924265</v>
+        <v>2.2072631554891746</v>
       </c>
       <c r="W24">
-        <v>0.9740611796137848</v>
+        <v>0.96470908899347729</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>2.2420285469738347E-2</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>-1.4443540003761909E-2</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>-2.0265201880372693E-3</v>
+        <v>1.8171710860239243E-3</v>
       </c>
       <c r="F25">
-        <v>8.2535637039212687E-3</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -2175,63 +2175,63 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>-3.5315671822918442E-2</v>
+        <v>-1.4918087652734755E-2</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>7.3502445551724051E-3</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>1.4243855789215306E-2</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>-1.9416698245420239E-2</v>
+        <v>-6.0339295881799929E-3</v>
       </c>
       <c r="O25">
-        <v>3.8931888805674206E-2</v>
+        <v>-4.1580267333865733E-3</v>
       </c>
       <c r="P25">
-        <v>-1.4371143568043776E-2</v>
+        <v>-2.028063378887179E-2</v>
       </c>
       <c r="Q25">
-        <v>4.611693670466795E-3</v>
+        <v>1.0832051109391076E-3</v>
       </c>
       <c r="R25">
-        <v>3.8105392349912698E-2</v>
+        <v>-8.9003211115158791E-3</v>
       </c>
       <c r="S25">
-        <v>1.0261456712862861E-2</v>
+        <v>2.0386460777596448E-2</v>
       </c>
       <c r="T25">
-        <v>2.1803034924040246E-2</v>
+        <v>9.6131603225869423E-3</v>
       </c>
       <c r="U25">
-        <v>-1.5146954018336814E-2</v>
+        <v>-4.5288427607179148E-3</v>
       </c>
       <c r="V25">
-        <v>2.2072631554891746</v>
+        <v>5.7963531951759952</v>
       </c>
       <c r="W25">
-        <v>0.96470908899347729</v>
+        <v>0.94380529312069394</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1.3515643908005696E-2</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1.8171710860239243E-3</v>
+        <v>-5.7950938551377795E-3</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2246,199 +2246,199 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>-1.4918087652734755E-2</v>
+        <v>-1.2958053078425076E-2</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>1.0517020214518764E-3</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>6.4050489478870874E-3</v>
       </c>
       <c r="N26">
-        <v>-6.0339295881799929E-3</v>
+        <v>-5.1213520734369519E-3</v>
       </c>
       <c r="O26">
-        <v>-4.1580267333865733E-3</v>
+        <v>-8.0926982316266774E-4</v>
       </c>
       <c r="P26">
-        <v>-2.028063378887179E-2</v>
+        <v>-1.141776170099402E-2</v>
       </c>
       <c r="Q26">
-        <v>1.0832051109391076E-3</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>-8.9003211115158791E-3</v>
+        <v>4.4463700420855394E-2</v>
       </c>
       <c r="S26">
-        <v>2.0386460777596448E-2</v>
+        <v>1.4313807605194304E-2</v>
       </c>
       <c r="T26">
-        <v>9.6131603225869423E-3</v>
+        <v>1.8553338513800924E-2</v>
       </c>
       <c r="U26">
-        <v>-4.5288427607179148E-3</v>
+        <v>-8.3375065113658296E-3</v>
       </c>
       <c r="V26">
-        <v>5.7963531951759952</v>
+        <v>3.2509507586980821</v>
       </c>
       <c r="W26">
-        <v>0.94380529312069394</v>
+        <v>0.95749325964682519</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>1.3515643908005696E-2</v>
+        <v>6.8094122720538013E-3</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>-5.7950938551377795E-3</v>
+        <v>4.7897081953184786E-3</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>-7.368074551140888E-4</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>-9.6604592529133757E-3</v>
       </c>
       <c r="J27">
-        <v>-1.2958053078425076E-2</v>
+        <v>-1.4125593997601946E-2</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1.0517020214518764E-3</v>
+        <v>1.3097786169054637E-2</v>
       </c>
       <c r="M27">
-        <v>6.4050489478870874E-3</v>
+        <v>2.6690315480410341E-3</v>
       </c>
       <c r="N27">
-        <v>-5.1213520734369519E-3</v>
+        <v>-1.5642418442441745E-2</v>
       </c>
       <c r="O27">
-        <v>-8.0926982316266774E-4</v>
+        <v>-3.3253515992149401E-3</v>
       </c>
       <c r="P27">
-        <v>-1.141776170099402E-2</v>
+        <v>-1.1042102363610801E-2</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>7.6865642315909104E-3</v>
       </c>
       <c r="R27">
-        <v>4.4463700420855394E-2</v>
+        <v>6.5381810653015642E-3</v>
       </c>
       <c r="S27">
-        <v>1.4313807605194304E-2</v>
+        <v>1.8016701344448684E-2</v>
       </c>
       <c r="T27">
-        <v>1.8553338513800924E-2</v>
+        <v>2.0320659909480138E-2</v>
       </c>
       <c r="U27">
-        <v>-8.3375065113658296E-3</v>
+        <v>-5.1803252504492242E-3</v>
       </c>
       <c r="V27">
-        <v>3.2509507586980821</v>
+        <v>4.8528903953399736</v>
       </c>
       <c r="W27">
-        <v>0.95749325964682519</v>
+        <v>0.98288779629156497</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>6.8094122720538013E-3</v>
+        <v>1.4093895839285386E-2</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>4.7897081953184786E-3</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>-7.368074551140888E-4</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>-9.6604592529133757E-3</v>
+        <v>-9.0095736895629986E-3</v>
       </c>
       <c r="J28">
-        <v>-1.4125593997601946E-2</v>
+        <v>-7.0579973307025052E-3</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1.3097786169054637E-2</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>2.6690315480410341E-3</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>-1.5642418442441745E-2</v>
+        <v>-2.6135154463031852E-3</v>
       </c>
       <c r="O28">
-        <v>-3.3253515992149401E-3</v>
+        <v>-1.8856739677069728E-2</v>
       </c>
       <c r="P28">
-        <v>-1.1042102363610801E-2</v>
+        <v>-6.5234012974732022E-3</v>
       </c>
       <c r="Q28">
-        <v>7.6865642315909104E-3</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>6.5381810653015642E-3</v>
+        <v>8.7903563751662046E-3</v>
       </c>
       <c r="S28">
-        <v>1.8016701344448684E-2</v>
+        <v>1.1399772449990365E-2</v>
       </c>
       <c r="T28">
-        <v>2.0320659909480138E-2</v>
+        <v>9.0039822335483844E-3</v>
       </c>
       <c r="U28">
-        <v>-5.1803252504492242E-3</v>
+        <v>0</v>
       </c>
       <c r="V28">
-        <v>4.8528903953399736</v>
+        <v>5.1041377941654655</v>
       </c>
       <c r="W28">
-        <v>0.98288779629156497</v>
+        <v>0.91444223040494466</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>1.4093895839285386E-2</v>
+        <v>8.6705011122111906E-3</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2456,10 +2456,10 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>-9.0095736895629986E-3</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>-7.0579973307025052E-3</v>
+        <v>-1.1377597819278815E-2</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2471,131 +2471,131 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>-2.6135154463031852E-3</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>-1.8856739677069728E-2</v>
+        <v>-3.0874171983817877E-4</v>
       </c>
       <c r="P29">
-        <v>-6.5234012974732022E-3</v>
+        <v>-4.9796346610432463E-3</v>
       </c>
       <c r="Q29">
         <v>0</v>
       </c>
       <c r="R29">
-        <v>8.7903563751662046E-3</v>
+        <v>1.0795203470299464E-2</v>
       </c>
       <c r="S29">
-        <v>1.1399772449990365E-2</v>
+        <v>5.5233475309720654E-3</v>
       </c>
       <c r="T29">
-        <v>9.0039822335483844E-3</v>
+        <v>4.2127927328659007E-3</v>
       </c>
       <c r="U29">
-        <v>0</v>
+        <v>-7.6671440680758473E-4</v>
       </c>
       <c r="V29">
-        <v>5.1041377941654655</v>
+        <v>2.6049500076025756</v>
       </c>
       <c r="W29">
-        <v>0.91444223040494466</v>
+        <v>0.93065554499098546</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1.6323297560500154E-2</v>
       </c>
       <c r="C30">
-        <v>8.6705011122111906E-3</v>
+        <v>2.1119911734823218E-2</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>-2.204655376142498E-3</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>-1.0990428108060744E-2</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>6.2686579078450018E-3</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>7.4575480201277454E-3</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>-1.1377597819278815E-2</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>-2.3013950005902669E-2</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>1.0100555133682153E-2</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>-6.3212241775743756E-3</v>
       </c>
       <c r="O30">
-        <v>-3.0874171983817877E-4</v>
+        <v>-3.5902690140077369E-3</v>
       </c>
       <c r="P30">
-        <v>-4.9796346610432463E-3</v>
+        <v>-1.7812687700667927E-2</v>
       </c>
       <c r="Q30">
-        <v>0</v>
+        <v>4.8484778315314126E-3</v>
       </c>
       <c r="R30">
-        <v>1.0795203470299464E-2</v>
+        <v>6.1732008598882011E-2</v>
       </c>
       <c r="S30">
-        <v>5.5233475309720654E-3</v>
+        <v>5.7107442244167264E-2</v>
       </c>
       <c r="T30">
-        <v>4.2127927328659007E-3</v>
+        <v>1.5157103310003715E-2</v>
       </c>
       <c r="U30">
-        <v>-7.6671440680758473E-4</v>
+        <v>-8.3793049888911918E-3</v>
       </c>
       <c r="V30">
-        <v>2.6049500076025756</v>
+        <v>1.3782549267393094</v>
       </c>
       <c r="W30">
-        <v>0.93065554499098546</v>
+        <v>0.96717048582469134</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31">
-        <v>1.6323297560500154E-2</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>2.1119911734823218E-2</v>
+        <v>1.5823422571326972E-2</v>
       </c>
       <c r="D31">
-        <v>-2.204655376142498E-3</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>-1.0990428108060744E-2</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>6.2686579078450018E-3</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>7.4575480201277454E-3</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2607,57 +2607,57 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>-2.3013950005902669E-2</v>
+        <v>-2.7448957801249225E-4</v>
       </c>
       <c r="M31">
-        <v>1.0100555133682153E-2</v>
+        <v>8.5507372277519814E-3</v>
       </c>
       <c r="N31">
-        <v>-6.3212241775743756E-3</v>
+        <v>1.130383680782688E-3</v>
       </c>
       <c r="O31">
-        <v>-3.5902690140077369E-3</v>
+        <v>5.4969487407197006E-3</v>
       </c>
       <c r="P31">
-        <v>-1.7812687700667927E-2</v>
+        <v>-8.7343914549751645E-3</v>
       </c>
       <c r="Q31">
-        <v>4.8484778315314126E-3</v>
+        <v>2.5174804049306297E-3</v>
       </c>
       <c r="R31">
-        <v>6.1732008598882011E-2</v>
+        <v>3.0847144567556141E-2</v>
       </c>
       <c r="S31">
-        <v>5.7107442244167264E-2</v>
+        <v>1.237668378552558E-2</v>
       </c>
       <c r="T31">
-        <v>1.5157103310003715E-2</v>
+        <v>6.4662797578950767E-3</v>
       </c>
       <c r="U31">
-        <v>-8.3793049888911918E-3</v>
+        <v>0</v>
       </c>
       <c r="V31">
-        <v>1.3782549267393094</v>
+        <v>-0.30284879341693305</v>
       </c>
       <c r="W31">
-        <v>0.96717048582469134</v>
+        <v>0.94035407419789663</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>1.5823422571326972E-2</v>
+        <v>1.0640331570290738E-2</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>-1.2403514067956024E-2</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2678,57 +2678,57 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>-2.7448957801249225E-4</v>
+        <v>-1.2865297620110653E-2</v>
       </c>
       <c r="M32">
-        <v>8.5507372277519814E-3</v>
+        <v>8.3088367150295876E-3</v>
       </c>
       <c r="N32">
-        <v>1.130383680782688E-3</v>
+        <v>-1.1095927476914654E-2</v>
       </c>
       <c r="O32">
-        <v>5.4969487407197006E-3</v>
+        <v>4.1224329986254256E-2</v>
       </c>
       <c r="P32">
-        <v>-8.7343914549751645E-3</v>
+        <v>-1.8702518916095028E-2</v>
       </c>
       <c r="Q32">
-        <v>2.5174804049306297E-3</v>
+        <v>-5.5992049547537762E-4</v>
       </c>
       <c r="R32">
-        <v>3.0847144567556141E-2</v>
+        <v>4.8376269481278149E-2</v>
       </c>
       <c r="S32">
-        <v>1.237668378552558E-2</v>
+        <v>1.2512437387526379E-2</v>
       </c>
       <c r="T32">
-        <v>6.4662797578950767E-3</v>
+        <v>2.508458602256625E-2</v>
       </c>
       <c r="U32">
-        <v>0</v>
+        <v>-4.8988181699142807E-3</v>
       </c>
       <c r="V32">
-        <v>-0.30284879341693305</v>
+        <v>9.4642021379121921E-2</v>
       </c>
       <c r="W32">
-        <v>0.94035407419789663</v>
+        <v>0.96051277568218407</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>1.0640331570290738E-2</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>-1.2403514067956024E-2</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2749,45 +2749,45 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>-1.2865297620110653E-2</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>8.3088367150295876E-3</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>-1.1095927476914654E-2</v>
+        <v>-1.5627915788822812E-2</v>
       </c>
       <c r="O33">
-        <v>4.1224329986254256E-2</v>
+        <v>-1.2956432616844496E-2</v>
       </c>
       <c r="P33">
-        <v>-1.8702518916095028E-2</v>
+        <v>-5.0437891817208961E-3</v>
       </c>
       <c r="Q33">
-        <v>-5.5992049547537762E-4</v>
+        <v>0</v>
       </c>
       <c r="R33">
-        <v>4.8376269481278149E-2</v>
+        <v>-2.095134880950744E-3</v>
       </c>
       <c r="S33">
-        <v>1.2512437387526379E-2</v>
+        <v>5.2401150314137805E-3</v>
       </c>
       <c r="T33">
-        <v>2.508458602256625E-2</v>
+        <v>0</v>
       </c>
       <c r="U33">
-        <v>-4.8988181699142807E-3</v>
+        <v>0</v>
       </c>
       <c r="V33">
-        <v>9.4642021379121921E-2</v>
+        <v>7.7804213086335903</v>
       </c>
       <c r="W33">
-        <v>0.96051277568218407</v>
+        <v>0.90817507843277767</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -2796,10 +2796,10 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>3.3779789711023676E-3</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>-4.5552586366855649E-3</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2814,63 +2814,63 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>-5.9983442292888085E-3</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>-1.461604210304464E-2</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34">
-        <v>-1.5627915788822812E-2</v>
+        <v>-6.5192389148628939E-3</v>
       </c>
       <c r="O34">
-        <v>-1.2956432616844496E-2</v>
+        <v>1.903170185076352E-2</v>
       </c>
       <c r="P34">
-        <v>-5.0437891817208961E-3</v>
+        <v>-9.7955408706343703E-3</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>8.0801044646765224E-3</v>
       </c>
       <c r="R34">
-        <v>-2.095134880950744E-3</v>
+        <v>3.3083654624753912E-2</v>
       </c>
       <c r="S34">
-        <v>5.2401150314137805E-3</v>
+        <v>2.4872820500846826E-2</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>1.4257093299715336E-2</v>
       </c>
       <c r="U34">
-        <v>0</v>
+        <v>-8.7918804340363262E-3</v>
       </c>
       <c r="V34">
-        <v>7.7804213086335903</v>
+        <v>2.3412774486266121</v>
       </c>
       <c r="W34">
-        <v>0.90817507843277767</v>
+        <v>0.95727282256787805</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1.5823397954186871E-2</v>
       </c>
       <c r="D35">
-        <v>3.3779789711023676E-3</v>
+        <v>-2.2863453092772639E-3</v>
       </c>
       <c r="E35">
-        <v>-4.5552586366855649E-3</v>
+        <v>-4.8605871610890678E-3</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2885,63 +2885,63 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>-5.9983442292888085E-3</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>-1.461604210304464E-2</v>
+        <v>-8.8257728408356415E-3</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>1.0248470490245373E-2</v>
       </c>
       <c r="N35">
-        <v>-6.5192389148628939E-3</v>
+        <v>8.9401105721902269E-3</v>
       </c>
       <c r="O35">
-        <v>1.903170185076352E-2</v>
+        <v>5.6459580889031405E-3</v>
       </c>
       <c r="P35">
-        <v>-9.7955408706343703E-3</v>
+        <v>-2.6190092136240326E-2</v>
       </c>
       <c r="Q35">
-        <v>8.0801044646765224E-3</v>
+        <v>7.1124042479405692E-3</v>
       </c>
       <c r="R35">
-        <v>3.3083654624753912E-2</v>
+        <v>4.4288401265491044E-2</v>
       </c>
       <c r="S35">
-        <v>2.4872820500846826E-2</v>
+        <v>3.5371658622205988E-2</v>
       </c>
       <c r="T35">
-        <v>1.4257093299715336E-2</v>
+        <v>3.618145272322864E-2</v>
       </c>
       <c r="U35">
-        <v>-8.7918804340363262E-3</v>
+        <v>0</v>
       </c>
       <c r="V35">
-        <v>2.3412774486266121</v>
+        <v>1.3484680524882986</v>
       </c>
       <c r="W35">
-        <v>0.95727282256787805</v>
+        <v>0.97497312554729809</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36">
-        <v>1.5823397954186871E-2</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>-2.2863453092772639E-3</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>-4.8605871610890678E-3</v>
+        <v>0</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2956,193 +2956,193 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>-3.1268493865125686E-3</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>-2.7668082848600673E-3</v>
       </c>
       <c r="L36">
-        <v>-8.8257728408356415E-3</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>1.0248470490245373E-2</v>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>8.9401105721902269E-3</v>
+        <v>-4.2114190568715067E-3</v>
       </c>
       <c r="O36">
-        <v>5.6459580889031405E-3</v>
+        <v>-7.7216375361070441E-3</v>
       </c>
       <c r="P36">
-        <v>-2.6190092136240326E-2</v>
+        <v>-8.1986678997442478E-4</v>
       </c>
       <c r="Q36">
-        <v>7.1124042479405692E-3</v>
+        <v>0</v>
       </c>
       <c r="R36">
-        <v>4.4288401265491044E-2</v>
+        <v>0</v>
       </c>
       <c r="S36">
-        <v>3.5371658622205988E-2</v>
+        <v>0</v>
       </c>
       <c r="T36">
-        <v>3.618145272322864E-2</v>
+        <v>2.9500608174756822E-3</v>
       </c>
       <c r="U36">
         <v>0</v>
       </c>
       <c r="V36">
-        <v>1.3484680524882986</v>
+        <v>3.6286072762214707</v>
       </c>
       <c r="W36">
-        <v>0.97497312554729809</v>
+        <v>0.70320330185854885</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1.8124663821397534E-3</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1.3660359351660245E-2</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>-1.9389289087826688E-3</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>8.1878959760631491E-4</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>7.4521808660275854E-7</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>-1.3177395674680011E-2</v>
       </c>
       <c r="J37">
-        <v>-3.1268493865125686E-3</v>
+        <v>-3.6285067357901948E-2</v>
       </c>
       <c r="K37">
-        <v>-2.7668082848600673E-3</v>
+        <v>1.4704377323197095E-2</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>2.6276630698506644E-3</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37">
-        <v>-4.2114190568715067E-3</v>
+        <v>-7.2048497126356676E-3</v>
       </c>
       <c r="O37">
-        <v>-7.7216375361070441E-3</v>
+        <v>-2.9036149423535503E-3</v>
       </c>
       <c r="P37">
-        <v>-8.1986678997442478E-4</v>
+        <v>-2.3719890325206183E-3</v>
       </c>
       <c r="Q37">
         <v>0</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>3.389064517168737E-2</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>6.9943343037723784E-3</v>
       </c>
       <c r="T37">
-        <v>2.9500608174756822E-3</v>
+        <v>2.6929169070971086E-2</v>
       </c>
       <c r="U37">
-        <v>0</v>
+        <v>1.4785823526779964E-3</v>
       </c>
       <c r="V37">
-        <v>3.6286072762214707</v>
+        <v>5.0347420523578048</v>
       </c>
       <c r="W37">
-        <v>0.70320330185854885</v>
+        <v>0.9660160610795866</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38">
-        <v>1.8124663821397534E-3</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1.3660359351660245E-2</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>-1.9389289087826688E-3</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38">
-        <v>8.1878959760631491E-4</v>
+        <v>0</v>
       </c>
       <c r="H38">
-        <v>7.4521808660275854E-7</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>-1.3177395674680011E-2</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>-3.6285067357901948E-2</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>1.4704377323197095E-2</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>2.6276630698506644E-3</v>
+        <v>0</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38">
-        <v>-7.2048497126356676E-3</v>
+        <v>-1.7210269908289919E-2</v>
       </c>
       <c r="O38">
-        <v>-2.9036149423535503E-3</v>
+        <v>7.8145911068505294E-3</v>
       </c>
       <c r="P38">
-        <v>-2.3719890325206183E-3</v>
+        <v>-6.2237111305683086E-3</v>
       </c>
       <c r="Q38">
         <v>0</v>
       </c>
       <c r="R38">
-        <v>3.389064517168737E-2</v>
+        <v>-4.9207691825353178E-3</v>
       </c>
       <c r="S38">
-        <v>6.9943343037723784E-3</v>
+        <v>1.6904691472070993E-2</v>
       </c>
       <c r="T38">
-        <v>2.6929169070971086E-2</v>
+        <v>8.2933107501889178E-3</v>
       </c>
       <c r="U38">
-        <v>1.4785823526779964E-3</v>
+        <v>0</v>
       </c>
       <c r="V38">
-        <v>5.0347420523578048</v>
+        <v>4.0372350219885522</v>
       </c>
       <c r="W38">
-        <v>0.9660160610795866</v>
+        <v>0.89892351574093543</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3151,152 +3151,152 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>-2.9226449826137224E-3</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>-5.8932809972320017E-3</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>-1.3596464163351104E-3</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>9.4129970220980022E-4</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>-1.3513430591205319E-2</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>-1.4887318418714572E-2</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>1.2900991933698458E-2</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>3.1423902425125015E-3</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39">
-        <v>-1.7210269908289919E-2</v>
+        <v>4.1936743070737853E-3</v>
       </c>
       <c r="O39">
-        <v>7.8145911068505294E-3</v>
+        <v>-1.519481394399579E-3</v>
       </c>
       <c r="P39">
-        <v>-6.2237111305683086E-3</v>
+        <v>-2.2348358894691778E-2</v>
       </c>
       <c r="Q39">
-        <v>0</v>
+        <v>-8.8211725091031116E-4</v>
       </c>
       <c r="R39">
-        <v>-4.9207691825353178E-3</v>
+        <v>3.233556397142149E-2</v>
       </c>
       <c r="S39">
-        <v>1.6904691472070993E-2</v>
+        <v>2.7329288362661391E-2</v>
       </c>
       <c r="T39">
-        <v>8.2933107501889178E-3</v>
+        <v>1.2673043663068571E-2</v>
       </c>
       <c r="U39">
-        <v>0</v>
+        <v>-4.1562931925230012E-3</v>
       </c>
       <c r="V39">
-        <v>4.0372350219885522</v>
+        <v>6.0801328247210984</v>
       </c>
       <c r="W39">
-        <v>0.89892351574093543</v>
+        <v>0.98212593334995901</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>7.2194920724771971E-3</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>5.5694507503860147E-3</v>
       </c>
       <c r="D40">
-        <v>-2.9226449826137224E-3</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>-5.8932809972320017E-3</v>
+        <v>-2.6788644139070375E-3</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>-1.3596464163351104E-3</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>9.4129970220980022E-4</v>
+        <v>2.1625575038003086E-3</v>
       </c>
       <c r="I40">
-        <v>-1.3513430591205319E-2</v>
+        <v>-1.3996161217503899E-2</v>
       </c>
       <c r="J40">
-        <v>-1.4887318418714572E-2</v>
+        <v>-2.3482248330560396E-2</v>
       </c>
       <c r="K40">
-        <v>1.2900991933698458E-2</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>3.1423902425125015E-3</v>
+        <v>-1.3407658495316428E-3</v>
       </c>
       <c r="M40">
-        <v>0</v>
+        <v>8.7584420232467222E-3</v>
       </c>
       <c r="N40">
-        <v>4.1936743070737853E-3</v>
+        <v>-2.2939958280703016E-2</v>
       </c>
       <c r="O40">
-        <v>-1.519481394399579E-3</v>
+        <v>2.1844108923776411E-2</v>
       </c>
       <c r="P40">
-        <v>-2.2348358894691778E-2</v>
+        <v>-1.0585957683863455E-2</v>
       </c>
       <c r="Q40">
-        <v>-8.8211725091031116E-4</v>
+        <v>-2.758087626571648E-4</v>
       </c>
       <c r="R40">
-        <v>3.233556397142149E-2</v>
+        <v>2.6857545052329741E-2</v>
       </c>
       <c r="S40">
-        <v>2.7329288362661391E-2</v>
+        <v>7.6117894471693578E-3</v>
       </c>
       <c r="T40">
-        <v>1.2673043663068571E-2</v>
+        <v>4.8206798282644479E-3</v>
       </c>
       <c r="U40">
-        <v>-4.1562931925230012E-3</v>
+        <v>-3.7649289909360457E-3</v>
       </c>
       <c r="V40">
-        <v>6.0801328247210984</v>
+        <v>4.3521551121673641</v>
       </c>
       <c r="W40">
-        <v>0.98212593334995901</v>
+        <v>0.94739044723934296</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B41">
-        <v>7.2194920724771971E-3</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>5.5694507503860147E-3</v>
+        <v>4.1523106809273111E-2</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>-2.6788644139070375E-3</v>
+        <v>-7.0835516089560232E-3</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -3305,69 +3305,69 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>2.1625575038003086E-3</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>-1.3996161217503899E-2</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>-2.3482248330560396E-2</v>
+        <v>-3.2818117663213735E-2</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>-1.3407658495316428E-3</v>
+        <v>3.2180676356775859E-3</v>
       </c>
       <c r="M41">
-        <v>8.7584420232467222E-3</v>
+        <v>2.445193952324266E-2</v>
       </c>
       <c r="N41">
-        <v>-2.2939958280703016E-2</v>
+        <v>-1.4911415930468769E-2</v>
       </c>
       <c r="O41">
-        <v>2.1844108923776411E-2</v>
+        <v>-1.4887531895185777E-3</v>
       </c>
       <c r="P41">
-        <v>-1.0585957683863455E-2</v>
+        <v>-1.7802475558664304E-2</v>
       </c>
       <c r="Q41">
-        <v>-2.758087626571648E-4</v>
+        <v>0</v>
       </c>
       <c r="R41">
-        <v>2.6857545052329741E-2</v>
+        <v>4.8552981831529313E-2</v>
       </c>
       <c r="S41">
-        <v>7.6117894471693578E-3</v>
+        <v>1.935292337807077E-2</v>
       </c>
       <c r="T41">
-        <v>4.8206798282644479E-3</v>
+        <v>1.5689690957229739E-2</v>
       </c>
       <c r="U41">
-        <v>-3.7649289909360457E-3</v>
+        <v>-5.6240089865602135E-3</v>
       </c>
       <c r="V41">
-        <v>4.3521551121673641</v>
+        <v>2.5938074664028301</v>
       </c>
       <c r="W41">
-        <v>0.94739044723934296</v>
+        <v>0.95151079716737952</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>5.0111927074928996E-3</v>
       </c>
       <c r="C42">
-        <v>4.1523106809273111E-2</v>
+        <v>3.0830683879568083E-2</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>-3.3577299102380605E-3</v>
       </c>
       <c r="E42">
-        <v>-7.0835516089560232E-3</v>
+        <v>-4.4646718164316219E-3</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -3382,63 +3382,63 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>-3.2818117663213735E-2</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>0</v>
+        <v>-1.2806517146298822E-2</v>
       </c>
       <c r="L42">
-        <v>3.2180676356775859E-3</v>
+        <v>-6.5420129981215193E-3</v>
       </c>
       <c r="M42">
-        <v>2.445193952324266E-2</v>
+        <v>3.7683264111894035E-3</v>
       </c>
       <c r="N42">
-        <v>-1.4911415930468769E-2</v>
+        <v>-1.0885511479220697E-2</v>
       </c>
       <c r="O42">
-        <v>-1.4887531895185777E-3</v>
+        <v>-1.436926655302566E-2</v>
       </c>
       <c r="P42">
-        <v>-1.7802475558664304E-2</v>
+        <v>-1.5859816052682697E-2</v>
       </c>
       <c r="Q42">
-        <v>0</v>
+        <v>1.8722023074904011E-3</v>
       </c>
       <c r="R42">
-        <v>4.8552981831529313E-2</v>
+        <v>2.7331816270753213E-2</v>
       </c>
       <c r="S42">
-        <v>1.935292337807077E-2</v>
+        <v>2.4072426815754694E-2</v>
       </c>
       <c r="T42">
-        <v>1.5689690957229739E-2</v>
+        <v>1.8648273586319316E-2</v>
       </c>
       <c r="U42">
-        <v>-5.6240089865602135E-3</v>
+        <v>0</v>
       </c>
       <c r="V42">
-        <v>2.5938074664028301</v>
+        <v>3.4165986045400265</v>
       </c>
       <c r="W42">
-        <v>0.95151079716737952</v>
+        <v>0.96385239097508557</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43">
-        <v>5.0111927074928996E-3</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>3.0830683879568083E-2</v>
+        <v>1.6571552143050707E-2</v>
       </c>
       <c r="D43">
-        <v>-3.3577299102380605E-3</v>
+        <v>9.7656307189599432E-4</v>
       </c>
       <c r="E43">
-        <v>-4.4646718164316219E-3</v>
+        <v>-2.9593114325405919E-3</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -3447,69 +3447,69 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>2.3611292282422671E-3</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>-5.9080238503074218E-3</v>
       </c>
       <c r="K43">
-        <v>-1.2806517146298822E-2</v>
+        <v>-3.1452842733480178E-3</v>
       </c>
       <c r="L43">
-        <v>-6.5420129981215193E-3</v>
+        <v>0</v>
       </c>
       <c r="M43">
-        <v>3.7683264111894035E-3</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>-1.0885511479220697E-2</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>-1.436926655302566E-2</v>
+        <v>-9.402433194984617E-3</v>
       </c>
       <c r="P43">
-        <v>-1.5859816052682697E-2</v>
+        <v>1.0324465714663009E-3</v>
       </c>
       <c r="Q43">
-        <v>1.8722023074904011E-3</v>
+        <v>0</v>
       </c>
       <c r="R43">
-        <v>2.7331816270753213E-2</v>
+        <v>1.2466341742849793E-2</v>
       </c>
       <c r="S43">
-        <v>2.4072426815754694E-2</v>
+        <v>9.6231260463687735E-4</v>
       </c>
       <c r="T43">
-        <v>1.8648273586319316E-2</v>
+        <v>4.7624163029029816E-3</v>
       </c>
       <c r="U43">
         <v>0</v>
       </c>
       <c r="V43">
-        <v>3.4165986045400265</v>
+        <v>2.4300419065406338</v>
       </c>
       <c r="W43">
-        <v>0.96385239097508557</v>
+        <v>0.83347815319170304</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>1.6571552143050707E-2</v>
+        <v>3.3211536093226871E-2</v>
       </c>
       <c r="D44">
-        <v>9.7656307189599432E-4</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>-2.9593114325405919E-3</v>
+        <v>-2.5682395930461841E-3</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -3518,69 +3518,69 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>2.3611292282422671E-3</v>
+        <v>4.9140351611011573E-3</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>-5.9080238503074218E-3</v>
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>-3.1452842733480178E-3</v>
+        <v>0</v>
       </c>
       <c r="L44">
-        <v>0</v>
+        <v>4.7050054815585707E-3</v>
       </c>
       <c r="M44">
-        <v>0</v>
+        <v>6.434166959852528E-3</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>1.1097371878295073E-3</v>
       </c>
       <c r="O44">
-        <v>-9.402433194984617E-3</v>
+        <v>-1.4295359778019484E-3</v>
       </c>
       <c r="P44">
-        <v>1.0324465714663009E-3</v>
+        <v>-2.9264913415304586E-2</v>
       </c>
       <c r="Q44">
-        <v>0</v>
+        <v>-5.3931050354313276E-3</v>
       </c>
       <c r="R44">
-        <v>1.2466341742849793E-2</v>
+        <v>2.6092817234012647E-2</v>
       </c>
       <c r="S44">
-        <v>9.6231260463687735E-4</v>
+        <v>6.4487600069451194E-3</v>
       </c>
       <c r="T44">
-        <v>4.7624163029029816E-3</v>
+        <v>2.4411942686374154E-2</v>
       </c>
       <c r="U44">
         <v>0</v>
       </c>
       <c r="V44">
-        <v>2.4300419065406338</v>
+        <v>1.8201709021194254</v>
       </c>
       <c r="W44">
-        <v>0.83347815319170304</v>
+        <v>0.97187377507000705</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>3.3211536093226871E-2</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>-2.551536729241463E-4</v>
       </c>
       <c r="E45">
-        <v>-2.5682395930461841E-3</v>
+        <v>-1.1793003271530996E-3</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3589,72 +3589,72 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>4.9140351611011573E-3</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>-1.9792064488378065E-2</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>4.7050054815585707E-3</v>
+        <v>0</v>
       </c>
       <c r="M45">
-        <v>6.434166959852528E-3</v>
+        <v>0</v>
       </c>
       <c r="N45">
-        <v>1.1097371878295073E-3</v>
+        <v>-7.4907107091043389E-3</v>
       </c>
       <c r="O45">
-        <v>-1.4295359778019484E-3</v>
+        <v>0</v>
       </c>
       <c r="P45">
-        <v>-2.9264913415304586E-2</v>
+        <v>-1.1070040280826636E-2</v>
       </c>
       <c r="Q45">
-        <v>-5.3931050354313276E-3</v>
+        <v>2.3161817647456896E-3</v>
       </c>
       <c r="R45">
-        <v>2.6092817234012647E-2</v>
+        <v>-7.4133750707112761E-4</v>
       </c>
       <c r="S45">
-        <v>6.4487600069451194E-3</v>
+        <v>1.2219540317247268E-2</v>
       </c>
       <c r="T45">
-        <v>2.4411942686374154E-2</v>
+        <v>1.771708455612795E-2</v>
       </c>
       <c r="U45">
-        <v>0</v>
+        <v>-1.217848122143046E-2</v>
       </c>
       <c r="V45">
-        <v>1.8201709021194254</v>
+        <v>6.646632772865936</v>
       </c>
       <c r="W45">
-        <v>0.97187377507000705</v>
+        <v>0.96582653144863162</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>2.2874620903157103E-2</v>
       </c>
       <c r="D46">
-        <v>-2.551536729241463E-4</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>-1.1793003271530996E-3</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>4.2952601839588668E-3</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3666,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>-1.9792064488378065E-2</v>
+        <v>-2.095592538235045E-2</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -3678,45 +3678,45 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>-7.4907107091043389E-3</v>
+        <v>-4.9588434111014741E-3</v>
       </c>
       <c r="O46">
-        <v>0</v>
+        <v>-1.6248627681377054E-2</v>
       </c>
       <c r="P46">
-        <v>-1.1070040280826636E-2</v>
+        <v>-5.7902634045709951E-3</v>
       </c>
       <c r="Q46">
-        <v>2.3161817647456896E-3</v>
+        <v>0</v>
       </c>
       <c r="R46">
-        <v>-7.4133750707112761E-4</v>
+        <v>1.9226255329159768E-3</v>
       </c>
       <c r="S46">
-        <v>1.2219540317247268E-2</v>
+        <v>7.4666184911053425E-3</v>
       </c>
       <c r="T46">
-        <v>1.771708455612795E-2</v>
+        <v>1.3768425344462079E-2</v>
       </c>
       <c r="U46">
-        <v>-1.217848122143046E-2</v>
+        <v>0</v>
       </c>
       <c r="V46">
-        <v>6.646632772865936</v>
+        <v>4.4508229336250551</v>
       </c>
       <c r="W46">
-        <v>0.96582653144863162</v>
+        <v>0.92908166443848017</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>5.6768154574238904E-3</v>
       </c>
       <c r="C47">
-        <v>2.2874620903157103E-2</v>
+        <v>1.2187344610584188E-2</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -3725,7 +3725,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>4.2952601839588668E-3</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -3737,60 +3737,60 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>-2.095592538235045E-2</v>
+        <v>-5.7930735117213278E-3</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>-3.6805014868162328E-3</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>2.1777620310249723E-3</v>
       </c>
       <c r="M47">
-        <v>0</v>
+        <v>2.5686777686689754E-3</v>
       </c>
       <c r="N47">
-        <v>-4.9588434111014741E-3</v>
+        <v>-5.8844871862979388E-3</v>
       </c>
       <c r="O47">
-        <v>-1.6248627681377054E-2</v>
+        <v>-1.6555977854555419E-2</v>
       </c>
       <c r="P47">
-        <v>-5.7902634045709951E-3</v>
+        <v>-7.5172671623207439E-3</v>
       </c>
       <c r="Q47">
         <v>0</v>
       </c>
       <c r="R47">
-        <v>1.9226255329159768E-3</v>
+        <v>1.083051013373103E-2</v>
       </c>
       <c r="S47">
-        <v>7.4666184911053425E-3</v>
+        <v>3.0380729847260179E-3</v>
       </c>
       <c r="T47">
-        <v>1.3768425344462079E-2</v>
+        <v>9.1059678882075643E-3</v>
       </c>
       <c r="U47">
         <v>0</v>
       </c>
       <c r="V47">
-        <v>4.4508229336250551</v>
+        <v>3.3750125971943499</v>
       </c>
       <c r="W47">
-        <v>0.92908166443848017</v>
+        <v>0.92440526176071725</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48">
-        <v>5.6768154574238904E-3</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>1.2187344610584188E-2</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>-4.1900197730898757E-3</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -3808,51 +3808,51 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>-5.7930735117213278E-3</v>
+        <v>0</v>
       </c>
       <c r="K48">
-        <v>-3.6805014868162328E-3</v>
+        <v>0</v>
       </c>
       <c r="L48">
-        <v>2.1777620310249723E-3</v>
+        <v>-4.0668777978463306E-4</v>
       </c>
       <c r="M48">
-        <v>2.5686777686689754E-3</v>
+        <v>0</v>
       </c>
       <c r="N48">
-        <v>-5.8844871862979388E-3</v>
+        <v>-4.1132044231607569E-3</v>
       </c>
       <c r="O48">
-        <v>-1.6555977854555419E-2</v>
+        <v>-2.3401838515338842E-3</v>
       </c>
       <c r="P48">
-        <v>-7.5172671623207439E-3</v>
+        <v>-1.7930215756991708E-2</v>
       </c>
       <c r="Q48">
         <v>0</v>
       </c>
       <c r="R48">
-        <v>1.083051013373103E-2</v>
+        <v>9.0704810411393125E-3</v>
       </c>
       <c r="S48">
-        <v>3.0380729847260179E-3</v>
+        <v>8.0441452503362838E-3</v>
       </c>
       <c r="T48">
-        <v>9.1059678882075643E-3</v>
+        <v>1.1893008632243034E-2</v>
       </c>
       <c r="U48">
         <v>0</v>
       </c>
       <c r="V48">
-        <v>3.3750125971943499</v>
+        <v>4.6652440913676143</v>
       </c>
       <c r="W48">
-        <v>0.92440526176071725</v>
+        <v>0.97740992966411488</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -3861,10 +3861,10 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <v>-4.1900197730898757E-3</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>-6.9131283494993671E-3</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -3879,63 +3879,63 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>-1.0200734597693394E-2</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>-4.0668777978463306E-4</v>
+        <v>0</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
       <c r="N49">
-        <v>-4.1132044231607569E-3</v>
+        <v>-2.7116823666034568E-3</v>
       </c>
       <c r="O49">
-        <v>-2.3401838515338842E-3</v>
+        <v>7.143172523663522E-3</v>
       </c>
       <c r="P49">
-        <v>-1.7930215756991708E-2</v>
+        <v>-1.677674857842585E-2</v>
       </c>
       <c r="Q49">
-        <v>0</v>
+        <v>1.0829492607963282E-2</v>
       </c>
       <c r="R49">
-        <v>9.0704810411393125E-3</v>
+        <v>5.0732303960289383E-4</v>
       </c>
       <c r="S49">
-        <v>8.0441452503362838E-3</v>
+        <v>1.6820509474912881E-2</v>
       </c>
       <c r="T49">
-        <v>1.1893008632243034E-2</v>
+        <v>2.3456323501038993E-2</v>
       </c>
       <c r="U49">
         <v>0</v>
       </c>
       <c r="V49">
-        <v>4.6652440913676143</v>
+        <v>5.6684741059891159</v>
       </c>
       <c r="W49">
-        <v>0.97740992966411488</v>
+        <v>0.97203364107304235</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>9.5433684157661576E-3</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>-6.9131283494993671E-3</v>
+        <v>-3.6482461746888822E-3</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -3950,63 +3950,63 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>-1.0200734597693394E-2</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>-9.6020727403955831E-3</v>
       </c>
       <c r="L50">
         <v>0</v>
       </c>
       <c r="M50">
-        <v>0</v>
+        <v>1.6202751904564991E-3</v>
       </c>
       <c r="N50">
-        <v>-2.7116823666034568E-3</v>
+        <v>-8.1434078373189001E-3</v>
       </c>
       <c r="O50">
-        <v>7.143172523663522E-3</v>
+        <v>-1.1994996630314879E-2</v>
       </c>
       <c r="P50">
-        <v>-1.677674857842585E-2</v>
+        <v>-3.2196527809572866E-3</v>
       </c>
       <c r="Q50">
-        <v>1.0829492607963282E-2</v>
+        <v>0</v>
       </c>
       <c r="R50">
-        <v>5.0732303960289383E-4</v>
+        <v>2.0971055925639713E-2</v>
       </c>
       <c r="S50">
-        <v>1.6820509474912881E-2</v>
+        <v>9.7516862371924088E-3</v>
       </c>
       <c r="T50">
-        <v>2.3456323501038993E-2</v>
+        <v>7.5198309385954877E-3</v>
       </c>
       <c r="U50">
         <v>0</v>
       </c>
       <c r="V50">
-        <v>5.6684741059891159</v>
+        <v>5.1113856154033925</v>
       </c>
       <c r="W50">
-        <v>0.97203364107304235</v>
+        <v>0.91621707613815584</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>9.5433684157661576E-3</v>
+        <v>1.1666678220180133E-2</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>-3.6482461746888822E-3</v>
+        <v>-2.4362505067818119E-3</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -4024,113 +4024,42 @@
         <v>0</v>
       </c>
       <c r="K51">
-        <v>-9.6020727403955831E-3</v>
+        <v>0</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>-1.956320142652864E-3</v>
       </c>
       <c r="M51">
-        <v>1.6202751904564991E-3</v>
+        <v>0</v>
       </c>
       <c r="N51">
-        <v>-8.1434078373189001E-3</v>
+        <v>-2.6671848199898668E-3</v>
       </c>
       <c r="O51">
-        <v>-1.1994996630314879E-2</v>
+        <v>9.9966983315422659E-3</v>
       </c>
       <c r="P51">
-        <v>-3.2196527809572866E-3</v>
+        <v>-1.8748745449466298E-2</v>
       </c>
       <c r="Q51">
-        <v>0</v>
+        <v>1.2442595335960403E-3</v>
       </c>
       <c r="R51">
-        <v>2.0971055925639713E-2</v>
+        <v>3.3356817020350912E-2</v>
       </c>
       <c r="S51">
-        <v>9.7516862371924088E-3</v>
+        <v>2.035682301941949E-2</v>
       </c>
       <c r="T51">
-        <v>7.5198309385954877E-3</v>
+        <v>1.7218870696606929E-2</v>
       </c>
       <c r="U51">
         <v>0</v>
       </c>
       <c r="V51">
-        <v>5.1113856154033925</v>
+        <v>1.1230545494502921</v>
       </c>
       <c r="W51">
-        <v>0.91621707613815584</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>55</v>
-      </c>
-      <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <v>1.1666678220180133E-2</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>-2.4362505067818119E-3</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <v>-1.956320142652864E-3</v>
-      </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-      <c r="N52">
-        <v>-2.6671848199898668E-3</v>
-      </c>
-      <c r="O52">
-        <v>9.9966983315422659E-3</v>
-      </c>
-      <c r="P52">
-        <v>-1.8748745449466298E-2</v>
-      </c>
-      <c r="Q52">
-        <v>1.2442595335960403E-3</v>
-      </c>
-      <c r="R52">
-        <v>3.3356817020350912E-2</v>
-      </c>
-      <c r="S52">
-        <v>2.035682301941949E-2</v>
-      </c>
-      <c r="T52">
-        <v>1.7218870696606929E-2</v>
-      </c>
-      <c r="U52">
-        <v>0</v>
-      </c>
-      <c r="V52">
-        <v>1.1230545494502921</v>
-      </c>
-      <c r="W52">
         <v>0.97498532608735755</v>
       </c>
     </row>

</xml_diff>